<commit_message>
Added Tourbement Result Weighting (Critical!), time decay consistency, diamter scaling, and judge education
</commit_message>
<xml_diff>
--- a/woodchopping.xlsx
+++ b/woodchopping.xlsx
@@ -17,8 +17,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -47,6 +49,9 @@
       <sz val="8"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -56,7 +61,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -155,11 +160,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -186,6 +197,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1483,51 +1499,53 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H107"/>
+  <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="P95" sqref="P95"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
-  <cols>
-    <col width="15.54296875" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="14.453125" customWidth="1" min="3" max="3"/>
-    <col width="19" customWidth="1" min="4" max="4"/>
-    <col width="12.81640625" customWidth="1" min="5" max="5"/>
-    <col width="11.1796875" customWidth="1" min="6" max="6"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="14" t="inlineStr">
         <is>
           <t>CompetitorID</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="14" t="inlineStr">
         <is>
           <t>Event</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="14" t="inlineStr">
         <is>
           <t>Time (seconds)</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="14" t="inlineStr">
         <is>
           <t>Size (mm)</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="14" t="inlineStr">
         <is>
           <t>Species Code</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="14" t="inlineStr">
         <is>
           <t>Date</t>
+        </is>
+      </c>
+      <c r="G1" s="14" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="H1" s="14" t="inlineStr">
+        <is>
+          <t>Unnamed: 7</t>
         </is>
       </c>
     </row>
@@ -2634,7 +2652,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F49" s="10" t="n">
+      <c r="F49" s="16" t="n">
         <v>45864</v>
       </c>
     </row>
@@ -2660,7 +2678,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F50" s="10" t="n">
+      <c r="F50" s="16" t="n">
         <v>45864</v>
       </c>
     </row>
@@ -2686,7 +2704,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F51" s="10" t="n">
+      <c r="F51" s="16" t="n">
         <v>45136</v>
       </c>
     </row>
@@ -2712,7 +2730,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F52" s="10" t="n">
+      <c r="F52" s="16" t="n">
         <v>45136</v>
       </c>
     </row>
@@ -2738,7 +2756,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F53" s="10" t="n">
+      <c r="F53" s="16" t="n">
         <v>43672</v>
       </c>
     </row>
@@ -2764,7 +2782,7 @@
           <t>S06</t>
         </is>
       </c>
-      <c r="F54" s="10" t="n">
+      <c r="F54" s="16" t="n">
         <v>43616</v>
       </c>
     </row>
@@ -2790,7 +2808,7 @@
           <t>S06</t>
         </is>
       </c>
-      <c r="F55" s="10" t="n">
+      <c r="F55" s="16" t="n">
         <v>43616</v>
       </c>
     </row>
@@ -2816,7 +2834,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F56" s="10" t="n">
+      <c r="F56" s="16" t="n">
         <v>43308</v>
       </c>
     </row>
@@ -2842,7 +2860,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F57" s="10" t="n">
+      <c r="F57" s="16" t="n">
         <v>43308</v>
       </c>
     </row>
@@ -2868,7 +2886,7 @@
           <t>S06</t>
         </is>
       </c>
-      <c r="F58" s="10" t="n">
+      <c r="F58" s="16" t="n">
         <v>43253</v>
       </c>
     </row>
@@ -2894,7 +2912,7 @@
           <t>S06</t>
         </is>
       </c>
-      <c r="F59" s="10" t="n">
+      <c r="F59" s="16" t="n">
         <v>43253</v>
       </c>
     </row>
@@ -2920,7 +2938,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F60" s="10" t="n">
+      <c r="F60" s="16" t="n">
         <v>43279</v>
       </c>
     </row>
@@ -2946,7 +2964,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F61" s="10" t="n">
+      <c r="F61" s="16" t="n">
         <v>43279</v>
       </c>
     </row>
@@ -2972,7 +2990,7 @@
           <t>S06</t>
         </is>
       </c>
-      <c r="F62" s="10" t="n">
+      <c r="F62" s="16" t="n">
         <v>42889</v>
       </c>
     </row>
@@ -2998,7 +3016,7 @@
           <t>S06</t>
         </is>
       </c>
-      <c r="F63" s="10" t="n">
+      <c r="F63" s="16" t="n">
         <v>42889</v>
       </c>
     </row>
@@ -3024,7 +3042,7 @@
           <t>S06</t>
         </is>
       </c>
-      <c r="F64" s="10" t="n">
+      <c r="F64" s="16" t="n">
         <v>42525</v>
       </c>
     </row>
@@ -3050,7 +3068,7 @@
           <t>S06</t>
         </is>
       </c>
-      <c r="F65" s="10" t="n">
+      <c r="F65" s="16" t="n">
         <v>42525</v>
       </c>
     </row>
@@ -3076,7 +3094,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F66" s="10" t="n">
+      <c r="F66" s="16" t="n">
         <v>42175</v>
       </c>
     </row>
@@ -3102,7 +3120,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F67" s="10" t="n">
+      <c r="F67" s="16" t="n">
         <v>42175</v>
       </c>
     </row>
@@ -3128,7 +3146,7 @@
           <t>S06</t>
         </is>
       </c>
-      <c r="F68" s="10" t="n">
+      <c r="F68" s="16" t="n">
         <v>43616</v>
       </c>
     </row>
@@ -3154,7 +3172,7 @@
           <t>S06</t>
         </is>
       </c>
-      <c r="F69" s="10" t="n">
+      <c r="F69" s="16" t="n">
         <v>43616</v>
       </c>
     </row>
@@ -3180,7 +3198,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F70" s="10" t="n">
+      <c r="F70" s="16" t="n">
         <v>42167</v>
       </c>
     </row>
@@ -3206,7 +3224,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F71" s="10" t="n">
+      <c r="F71" s="16" t="n">
         <v>42167</v>
       </c>
     </row>
@@ -3232,7 +3250,7 @@
           <t>S06</t>
         </is>
       </c>
-      <c r="F72" s="10" t="n">
+      <c r="F72" s="16" t="n">
         <v>43616</v>
       </c>
     </row>
@@ -3258,7 +3276,7 @@
           <t>S06</t>
         </is>
       </c>
-      <c r="F73" s="10" t="n">
+      <c r="F73" s="16" t="n">
         <v>43616</v>
       </c>
     </row>
@@ -3284,7 +3302,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F74" s="10" t="n">
+      <c r="F74" s="16" t="n">
         <v>43672</v>
       </c>
     </row>
@@ -3310,7 +3328,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F75" s="10" t="n">
+      <c r="F75" s="16" t="n">
         <v>43672</v>
       </c>
     </row>
@@ -3336,7 +3354,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F76" s="10" t="n">
+      <c r="F76" s="16" t="n">
         <v>45136</v>
       </c>
     </row>
@@ -3362,7 +3380,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F77" s="10" t="n">
+      <c r="F77" s="16" t="n">
         <v>45136</v>
       </c>
     </row>
@@ -3388,7 +3406,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F78" s="10" t="n">
+      <c r="F78" s="16" t="n">
         <v>45499</v>
       </c>
     </row>
@@ -3414,7 +3432,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F79" s="10" t="n">
+      <c r="F79" s="16" t="n">
         <v>45499</v>
       </c>
     </row>
@@ -3440,7 +3458,7 @@
           <t>S06</t>
         </is>
       </c>
-      <c r="F80" s="10" t="n">
+      <c r="F80" s="16" t="n">
         <v>43616</v>
       </c>
     </row>
@@ -3466,7 +3484,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F81" s="10" t="n">
+      <c r="F81" s="16" t="n">
         <v>45864</v>
       </c>
     </row>
@@ -3492,7 +3510,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F82" s="10" t="n">
+      <c r="F82" s="16" t="n">
         <v>45864</v>
       </c>
     </row>
@@ -3518,7 +3536,7 @@
           <t>S10</t>
         </is>
       </c>
-      <c r="F83" s="10" t="n">
+      <c r="F83" s="16" t="n">
         <v>45524</v>
       </c>
     </row>
@@ -3544,7 +3562,7 @@
           <t>S10</t>
         </is>
       </c>
-      <c r="F84" s="10" t="n">
+      <c r="F84" s="16" t="n">
         <v>45087</v>
       </c>
     </row>
@@ -3570,7 +3588,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F85" s="10" t="n">
+      <c r="F85" s="16" t="n">
         <v>45499</v>
       </c>
     </row>
@@ -3596,7 +3614,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F86" s="10" t="n">
+      <c r="F86" s="16" t="n">
         <v>45499</v>
       </c>
     </row>
@@ -3622,7 +3640,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F87" s="10" t="n">
+      <c r="F87" s="16" t="n">
         <v>45135</v>
       </c>
     </row>
@@ -3648,7 +3666,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F88" s="10" t="n">
+      <c r="F88" s="16" t="n">
         <v>45135</v>
       </c>
     </row>
@@ -3674,7 +3692,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F89" s="10" t="n">
+      <c r="F89" s="16" t="n">
         <v>44765</v>
       </c>
     </row>
@@ -3700,7 +3718,7 @@
           <t>S01</t>
         </is>
       </c>
-      <c r="F90" s="10" t="n">
+      <c r="F90" s="16" t="n">
         <v>44765</v>
       </c>
     </row>
@@ -3726,7 +3744,7 @@
           <t>S05</t>
         </is>
       </c>
-      <c r="F91" s="10" t="n">
+      <c r="F91" s="16" t="n">
         <v>45966</v>
       </c>
     </row>
@@ -3752,7 +3770,7 @@
           <t>S09</t>
         </is>
       </c>
-      <c r="F92" s="10" t="n">
+      <c r="F92" s="16" t="n">
         <v>45410</v>
       </c>
     </row>
@@ -3778,7 +3796,7 @@
           <t>S08</t>
         </is>
       </c>
-      <c r="F93" s="10" t="n">
+      <c r="F93" s="16" t="n">
         <v>45417</v>
       </c>
     </row>
@@ -3804,7 +3822,7 @@
           <t>S08</t>
         </is>
       </c>
-      <c r="F94" s="10" t="n">
+      <c r="F94" s="16" t="n">
         <v>45612</v>
       </c>
     </row>
@@ -3830,7 +3848,7 @@
           <t>S03</t>
         </is>
       </c>
-      <c r="F95" s="10" t="n">
+      <c r="F95" s="16" t="n">
         <v>45742</v>
       </c>
     </row>
@@ -3971,7 +3989,7 @@
           <t>S09</t>
         </is>
       </c>
-      <c r="F101" s="10" t="n">
+      <c r="F101" s="16" t="n">
         <v>45973</v>
       </c>
     </row>
@@ -3997,7 +4015,7 @@
           <t>S09</t>
         </is>
       </c>
-      <c r="F102" s="10" t="n">
+      <c r="F102" s="16" t="n">
         <v>45977</v>
       </c>
     </row>
@@ -4020,7 +4038,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Ponderosa Pine</t>
+          <t>S05</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -4058,7 +4076,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Ponderosa Pine</t>
+          <t>S05</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -4096,7 +4114,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Ponderosa Pine</t>
+          <t>S05</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -4134,7 +4152,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Ponderosa Pine</t>
+          <t>S05</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -4172,7 +4190,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Ponderosa Pine</t>
+          <t>S05</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -4191,7 +4209,387 @@
         </is>
       </c>
     </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>45.65</v>
+      </c>
+      <c r="D108" t="n">
+        <v>275</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>S05</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>2025-12-28T03:19:05</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>Heat 1</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>SB-SB-Test-DEC28-Heat-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>C009</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>56.78</v>
+      </c>
+      <c r="D109" t="n">
+        <v>275</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>S05</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>2025-12-28T03:19:05</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>Heat 1</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>SB-SB-Test-DEC28-Heat-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>C008</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="D110" t="n">
+        <v>275</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>S05</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>2025-12-28T03:19:05</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>Heat 1</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>SB-SB-Test-DEC28-Heat-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>C001</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>48.8</v>
+      </c>
+      <c r="D111" t="n">
+        <v>275</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>S05</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>2025-12-28T03:19:05</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>Heat 1</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>SB-SB-Test-DEC28-Heat-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>C005</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>76.8</v>
+      </c>
+      <c r="D112" t="n">
+        <v>275</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>S05</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>2025-12-28T03:19:05</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>Heat 1</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>SB-SB-Test-DEC28-Heat-1</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>C003</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>56.7</v>
+      </c>
+      <c r="D113" t="n">
+        <v>275</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>S05</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>2025-12-28T03:21:34</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>Heat 2</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>SB-SB-Test-DEC28-Heat-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>C002</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>55.6</v>
+      </c>
+      <c r="D114" t="n">
+        <v>275</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>S05</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>2025-12-28T03:21:34</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>Heat 2</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>SB-SB-Test-DEC28-Heat-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>C007</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>67.8</v>
+      </c>
+      <c r="D115" t="n">
+        <v>275</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>S05</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>2025-12-28T03:21:34</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>Heat 2</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>SB-SB-Test-DEC28-Heat-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>C010</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>61.4</v>
+      </c>
+      <c r="D116" t="n">
+        <v>275</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>S05</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>2025-12-28T03:21:34</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>Heat 2</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>SB-SB-Test-DEC28-Heat-2</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>C006</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>SB</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>116.7</v>
+      </c>
+      <c r="D117" t="n">
+        <v>275</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>S05</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>2025-12-28T03:21:34</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>Heat 2</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>SB-SB-Test-DEC28-Heat-2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>